<commit_message>
Addition of debug switch, some housekeeping in OptRecursive and main entrypoint code.
</commit_message>
<xml_diff>
--- a/Java/Test OptRecursive/OptRecursive_Testbench/Excel_Files/outputOpt/P_old.xlsx
+++ b/Java/Test OptRecursive/OptRecursive_Testbench/Excel_Files/outputOpt/P_old.xlsx
@@ -63,13 +63,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>383.11219454032147</v>
+        <v>1.0</v>
       </c>
       <c r="B1" t="n">
-        <v>-354.62458568768875</v>
+        <v>0.0</v>
       </c>
       <c r="C1" t="n">
-        <v>-346.0794149482263</v>
+        <v>0.0</v>
       </c>
       <c r="D1" t="n">
         <v>0.0</v>
@@ -108,28 +108,28 @@
         <v>0.0</v>
       </c>
       <c r="P1" t="n">
-        <v>0.6408878054596783</v>
+        <v>0.0</v>
       </c>
       <c r="Q1" t="n">
-        <v>0.6408878054596783</v>
+        <v>0.0</v>
       </c>
       <c r="R1" t="n">
-        <v>0.6408878054596785</v>
+        <v>0.0</v>
       </c>
       <c r="S1" t="n">
-        <v>0.6408878054596783</v>
+        <v>0.0</v>
       </c>
       <c r="T1" t="n">
-        <v>0.42725853697311905</v>
+        <v>0.0</v>
       </c>
       <c r="U1" t="n">
-        <v>0.4272585369731191</v>
+        <v>0.0</v>
       </c>
       <c r="V1" t="n">
-        <v>0.4272585369731191</v>
+        <v>0.0</v>
       </c>
       <c r="W1" t="n">
-        <v>0.4272585369731192</v>
+        <v>0.0</v>
       </c>
       <c r="X1" t="n">
         <v>0.0</v>
@@ -137,13 +137,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-354.62458568768875</v>
+        <v>0.0</v>
       </c>
       <c r="B2" t="n">
-        <v>827.7743959194788</v>
+        <v>1.0</v>
       </c>
       <c r="C2" t="n">
-        <v>-191.49727627135192</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n">
         <v>0.0</v>
@@ -182,28 +182,28 @@
         <v>0.0</v>
       </c>
       <c r="P2" t="n">
-        <v>0.3546245856876889</v>
+        <v>0.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.35462458568768895</v>
+        <v>0.0</v>
       </c>
       <c r="R2" t="n">
-        <v>0.35462458568768895</v>
+        <v>0.0</v>
       </c>
       <c r="S2" t="n">
-        <v>0.35462458568768906</v>
+        <v>0.0</v>
       </c>
       <c r="T2" t="n">
-        <v>0.2364163904584591</v>
+        <v>0.0</v>
       </c>
       <c r="U2" t="n">
-        <v>0.23641639045845905</v>
+        <v>0.0</v>
       </c>
       <c r="V2" t="n">
-        <v>0.23641639045845902</v>
+        <v>0.0</v>
       </c>
       <c r="W2" t="n">
-        <v>0.2364163904584589</v>
+        <v>0.0</v>
       </c>
       <c r="X2" t="n">
         <v>0.0</v>
@@ -211,13 +211,13 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-346.0794149482263</v>
+        <v>0.0</v>
       </c>
       <c r="B3" t="n">
-        <v>-191.49727627135192</v>
+        <v>0.0</v>
       </c>
       <c r="C3" t="n">
-        <v>837.1171159279576</v>
+        <v>1.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
@@ -256,28 +256,28 @@
         <v>0.0</v>
       </c>
       <c r="P3" t="n">
-        <v>0.3460794149482266</v>
+        <v>0.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.3460794149482265</v>
+        <v>0.0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.3460794149482264</v>
+        <v>0.0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.3460794149482264</v>
+        <v>0.0</v>
       </c>
       <c r="T3" t="n">
-        <v>0.23071960996548418</v>
+        <v>0.0</v>
       </c>
       <c r="U3" t="n">
-        <v>0.23071960996548407</v>
+        <v>0.0</v>
       </c>
       <c r="V3" t="n">
-        <v>0.23071960996548407</v>
+        <v>0.0</v>
       </c>
       <c r="W3" t="n">
-        <v>0.23071960996548402</v>
+        <v>0.0</v>
       </c>
       <c r="X3" t="n">
         <v>0.0</v>
@@ -294,7 +294,7 @@
         <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="E4" t="n">
         <v>0.0</v>
@@ -371,7 +371,7 @@
         <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="F5" t="n">
         <v>0.0</v>
@@ -448,7 +448,7 @@
         <v>0.0</v>
       </c>
       <c r="F6" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="G6" t="n">
         <v>0.0</v>
@@ -525,7 +525,7 @@
         <v>0.0</v>
       </c>
       <c r="G7" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="H7" t="n">
         <v>0.0</v>
@@ -602,7 +602,7 @@
         <v>0.0</v>
       </c>
       <c r="H8" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="I8" t="n">
         <v>0.0</v>
@@ -679,7 +679,7 @@
         <v>0.0</v>
       </c>
       <c r="I9" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="J9" t="n">
         <v>0.0</v>
@@ -756,7 +756,7 @@
         <v>0.0</v>
       </c>
       <c r="J10" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="K10" t="n">
         <v>0.0</v>
@@ -833,7 +833,7 @@
         <v>0.0</v>
       </c>
       <c r="K11" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="L11" t="n">
         <v>0.0</v>
@@ -910,7 +910,7 @@
         <v>0.0</v>
       </c>
       <c r="L12" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="M12" t="n">
         <v>0.0</v>
@@ -987,7 +987,7 @@
         <v>0.0</v>
       </c>
       <c r="M13" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="N13" t="n">
         <v>0.0</v>
@@ -1064,7 +1064,7 @@
         <v>0.0</v>
       </c>
       <c r="N14" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="O14" t="n">
         <v>0.0</v>
@@ -1141,7 +1141,7 @@
         <v>0.0</v>
       </c>
       <c r="O15" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
       <c r="P15" t="n">
         <v>0.0</v>
@@ -1173,13 +1173,13 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.6408878054596784</v>
+        <v>0.0</v>
       </c>
       <c r="B16" t="n">
-        <v>0.35462458568768873</v>
+        <v>0.0</v>
       </c>
       <c r="C16" t="n">
-        <v>0.34607941494822647</v>
+        <v>0.0</v>
       </c>
       <c r="D16" t="n">
         <v>0.0</v>
@@ -1218,28 +1218,28 @@
         <v>0.0</v>
       </c>
       <c r="P16" t="n">
-        <v>1023.9993591121946</v>
+        <v>1.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>-6.408878054596785E-4</v>
+        <v>0.0</v>
       </c>
       <c r="R16" t="n">
-        <v>-6.408878054596786E-4</v>
+        <v>0.0</v>
       </c>
       <c r="S16" t="n">
-        <v>-6.408878054596787E-4</v>
+        <v>0.0</v>
       </c>
       <c r="T16" t="n">
-        <v>-4.2725853697311915E-4</v>
+        <v>0.0</v>
       </c>
       <c r="U16" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="V16" t="n">
-        <v>-4.272585369731189E-4</v>
+        <v>0.0</v>
       </c>
       <c r="W16" t="n">
-        <v>-4.27258536973119E-4</v>
+        <v>0.0</v>
       </c>
       <c r="X16" t="n">
         <v>0.0</v>
@@ -1247,13 +1247,13 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.6408878054596784</v>
+        <v>0.0</v>
       </c>
       <c r="B17" t="n">
-        <v>0.35462458568768884</v>
+        <v>0.0</v>
       </c>
       <c r="C17" t="n">
-        <v>0.3460794149482263</v>
+        <v>0.0</v>
       </c>
       <c r="D17" t="n">
         <v>0.0</v>
@@ -1292,28 +1292,28 @@
         <v>0.0</v>
       </c>
       <c r="P17" t="n">
-        <v>-6.408878054596787E-4</v>
+        <v>0.0</v>
       </c>
       <c r="Q17" t="n">
-        <v>1023.9993591121946</v>
+        <v>1.0</v>
       </c>
       <c r="R17" t="n">
-        <v>-6.408878054596785E-4</v>
+        <v>0.0</v>
       </c>
       <c r="S17" t="n">
-        <v>-6.408878054596787E-4</v>
+        <v>0.0</v>
       </c>
       <c r="T17" t="n">
-        <v>-4.272585369731189E-4</v>
+        <v>0.0</v>
       </c>
       <c r="U17" t="n">
-        <v>-4.2725853697311877E-4</v>
+        <v>0.0</v>
       </c>
       <c r="V17" t="n">
-        <v>-4.272585369731187E-4</v>
+        <v>0.0</v>
       </c>
       <c r="W17" t="n">
-        <v>-4.2725853697311855E-4</v>
+        <v>0.0</v>
       </c>
       <c r="X17" t="n">
         <v>0.0</v>
@@ -1321,13 +1321,13 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.6408878054596785</v>
+        <v>0.0</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3546245856876887</v>
+        <v>0.0</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3460794149482263</v>
+        <v>0.0</v>
       </c>
       <c r="D18" t="n">
         <v>0.0</v>
@@ -1366,28 +1366,28 @@
         <v>0.0</v>
       </c>
       <c r="P18" t="n">
-        <v>-6.408878054596786E-4</v>
+        <v>0.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>-6.408878054596787E-4</v>
+        <v>0.0</v>
       </c>
       <c r="R18" t="n">
-        <v>1023.9993591121946</v>
+        <v>1.0</v>
       </c>
       <c r="S18" t="n">
-        <v>-6.408878054596786E-4</v>
+        <v>0.0</v>
       </c>
       <c r="T18" t="n">
-        <v>-4.272585369731189E-4</v>
+        <v>0.0</v>
       </c>
       <c r="U18" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="V18" t="n">
-        <v>-4.2725853697311904E-4</v>
+        <v>0.0</v>
       </c>
       <c r="W18" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="X18" t="n">
         <v>0.0</v>
@@ -1395,13 +1395,13 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.6408878054596784</v>
+        <v>0.0</v>
       </c>
       <c r="B19" t="n">
-        <v>0.35462458568768873</v>
+        <v>0.0</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3460794149482264</v>
+        <v>0.0</v>
       </c>
       <c r="D19" t="n">
         <v>0.0</v>
@@ -1440,28 +1440,28 @@
         <v>0.0</v>
       </c>
       <c r="P19" t="n">
-        <v>-6.408878054596784E-4</v>
+        <v>0.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>-6.408878054596784E-4</v>
+        <v>0.0</v>
       </c>
       <c r="R19" t="n">
-        <v>-6.408878054596782E-4</v>
+        <v>0.0</v>
       </c>
       <c r="S19" t="n">
-        <v>1023.9993591121946</v>
+        <v>1.0</v>
       </c>
       <c r="T19" t="n">
-        <v>-4.272585369731189E-4</v>
+        <v>0.0</v>
       </c>
       <c r="U19" t="n">
-        <v>-4.27258536973119E-4</v>
+        <v>0.0</v>
       </c>
       <c r="V19" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="W19" t="n">
-        <v>-4.2725853697311877E-4</v>
+        <v>0.0</v>
       </c>
       <c r="X19" t="n">
         <v>0.0</v>
@@ -1469,13 +1469,13 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.42725853697311894</v>
+        <v>0.0</v>
       </c>
       <c r="B20" t="n">
-        <v>0.23641639045845916</v>
+        <v>0.0</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2307196099654842</v>
+        <v>0.0</v>
       </c>
       <c r="D20" t="n">
         <v>0.0</v>
@@ -1514,28 +1514,28 @@
         <v>0.0</v>
       </c>
       <c r="P20" t="n">
-        <v>-4.2725853697311904E-4</v>
+        <v>0.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>-4.2725853697311915E-4</v>
+        <v>0.0</v>
       </c>
       <c r="R20" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="S20" t="n">
-        <v>-4.27258536973119E-4</v>
+        <v>0.0</v>
       </c>
       <c r="T20" t="n">
-        <v>1023.9997151609753</v>
+        <v>1.0</v>
       </c>
       <c r="U20" t="n">
-        <v>-2.8483902464874583E-4</v>
+        <v>0.0</v>
       </c>
       <c r="V20" t="n">
-        <v>-2.8483902464874594E-4</v>
+        <v>0.0</v>
       </c>
       <c r="W20" t="n">
-        <v>-2.848390246487459E-4</v>
+        <v>0.0</v>
       </c>
       <c r="X20" t="n">
         <v>0.0</v>
@@ -1543,13 +1543,13 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.42725853697311894</v>
+        <v>0.0</v>
       </c>
       <c r="B21" t="n">
-        <v>0.2364163904584591</v>
+        <v>0.0</v>
       </c>
       <c r="C21" t="n">
-        <v>0.23071960996548413</v>
+        <v>0.0</v>
       </c>
       <c r="D21" t="n">
         <v>0.0</v>
@@ -1588,28 +1588,28 @@
         <v>0.0</v>
       </c>
       <c r="P21" t="n">
-        <v>-4.27258536973119E-4</v>
+        <v>0.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>-4.27258536973119E-4</v>
+        <v>0.0</v>
       </c>
       <c r="R21" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="S21" t="n">
-        <v>-4.27258536973119E-4</v>
+        <v>0.0</v>
       </c>
       <c r="T21" t="n">
-        <v>-2.8483902464874583E-4</v>
+        <v>0.0</v>
       </c>
       <c r="U21" t="n">
-        <v>1023.9997151609753</v>
+        <v>1.0</v>
       </c>
       <c r="V21" t="n">
-        <v>-2.848390246487459E-4</v>
+        <v>0.0</v>
       </c>
       <c r="W21" t="n">
-        <v>-2.848390246487459E-4</v>
+        <v>0.0</v>
       </c>
       <c r="X21" t="n">
         <v>0.0</v>
@@ -1617,13 +1617,13 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.42725853697311894</v>
+        <v>0.0</v>
       </c>
       <c r="B22" t="n">
-        <v>0.23641639045845916</v>
+        <v>0.0</v>
       </c>
       <c r="C22" t="n">
-        <v>0.23071960996548413</v>
+        <v>0.0</v>
       </c>
       <c r="D22" t="n">
         <v>0.0</v>
@@ -1662,28 +1662,28 @@
         <v>0.0</v>
       </c>
       <c r="P22" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="Q22" t="n">
-        <v>-4.2725853697311904E-4</v>
+        <v>0.0</v>
       </c>
       <c r="R22" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="S22" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="T22" t="n">
-        <v>-2.848390246487459E-4</v>
+        <v>0.0</v>
       </c>
       <c r="U22" t="n">
-        <v>-2.848390246487459E-4</v>
+        <v>0.0</v>
       </c>
       <c r="V22" t="n">
-        <v>1023.9997151609753</v>
+        <v>1.0</v>
       </c>
       <c r="W22" t="n">
-        <v>-2.848390246487459E-4</v>
+        <v>0.0</v>
       </c>
       <c r="X22" t="n">
         <v>0.0</v>
@@ -1691,13 +1691,13 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.42725853697311894</v>
+        <v>0.0</v>
       </c>
       <c r="B23" t="n">
-        <v>0.23641639045845916</v>
+        <v>0.0</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2307196099654842</v>
+        <v>0.0</v>
       </c>
       <c r="D23" t="n">
         <v>0.0</v>
@@ -1736,28 +1736,28 @@
         <v>0.0</v>
       </c>
       <c r="P23" t="n">
-        <v>-4.2725853697311893E-4</v>
+        <v>0.0</v>
       </c>
       <c r="Q23" t="n">
-        <v>-4.272585369731191E-4</v>
+        <v>0.0</v>
       </c>
       <c r="R23" t="n">
-        <v>-4.2725853697311904E-4</v>
+        <v>0.0</v>
       </c>
       <c r="S23" t="n">
-        <v>-4.2725853697311915E-4</v>
+        <v>0.0</v>
       </c>
       <c r="T23" t="n">
-        <v>-2.8483902464874594E-4</v>
+        <v>0.0</v>
       </c>
       <c r="U23" t="n">
-        <v>-2.84839024648746E-4</v>
+        <v>0.0</v>
       </c>
       <c r="V23" t="n">
-        <v>-2.84839024648746E-4</v>
+        <v>0.0</v>
       </c>
       <c r="W23" t="n">
-        <v>1023.9997151609753</v>
+        <v>1.0</v>
       </c>
       <c r="X23" t="n">
         <v>0.0</v>
@@ -1834,7 +1834,7 @@
         <v>0.0</v>
       </c>
       <c r="X24" t="n">
-        <v>1024.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>